<commit_message>
Add new raw datasets. Start to prepare and cleansing the data to rigtht format.
</commit_message>
<xml_diff>
--- a/datasets/raw/databoks-aug-2022.xlsx
+++ b/datasets/raw/databoks-aug-2022.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PF1ZKYBY\Documents\alvin-project\minimum-wage-idn\indonesia-provinces-minimum-wage\datasets\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4393E95A-A6BA-4850-8BBC-1A708CB378DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="amCharts" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>nama_data</t>
-  </si>
-  <si>
-    <t>value</t>
   </si>
   <si>
     <t>DKI Jakarta</t>
@@ -125,8 +133,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,13 +164,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -487,297 +503,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2">
         <v>4641854</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>3561932</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3310723</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>3264884</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>3200000</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>3166460</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>3165876</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>3144446</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>3050172</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>3016738</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>3014497</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>2938564</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>2922516</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>2906473</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>2862231</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>2800580</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>2729463</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>2710596</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>2698941</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>2678863</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>2619313</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>2522610</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>2516971</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>2512539</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>2501203</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>2440486</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>2434328</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>2390739</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>2238094</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>2207212</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>1975000</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>1891567</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>1841487</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>1840916</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>1812935</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>